<commit_message>
forster voyage for square brackets
</commit_message>
<xml_diff>
--- a/Class-Examples/Regex/classDates/Fa2020SemesterDates.xlsx
+++ b/Class-Examples/Regex/classDates/Fa2020SemesterDates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eeb4/Documents/GitHub/newtfire/textEncoding-Hub/Class-Examples/Regex/classDates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1C161A4-CEEB-454C-B8E7-97F277B49548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2FDC47-079D-5749-B9B8-951C67F4A334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8000" yWindow="460" windowWidth="20800" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="5">
   <si>
     <t>M</t>
   </si>
@@ -396,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection sqref="A1:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -409,7 +409,7 @@
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>44067</v>
       </c>
@@ -422,14 +422,9 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1">
-        <v>43836</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f>A1+2</f>
         <v>44069</v>
@@ -443,14 +438,9 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
-        <v>43475</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>A2+2</f>
         <v>44071</v>
@@ -465,15 +455,9 @@
       <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G8" si="0">G1+7</f>
-        <v>43843</v>
-      </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>A1+7</f>
         <v>44074</v>
@@ -488,15 +472,9 @@
       <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1">
-        <f t="shared" si="0"/>
-        <v>43482</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f>A2+7</f>
         <v>44076</v>
@@ -505,21 +483,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:D32" si="1">D3+7</f>
+        <f t="shared" ref="D5:D32" si="0">D3+7</f>
         <v>44082</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1">
-        <f t="shared" si="0"/>
-        <v>43850</v>
-      </c>
-      <c r="H5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>A3+7</f>
         <v>44078</v>
@@ -528,603 +500,459 @@
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44084</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
-        <f t="shared" si="0"/>
-        <v>43489</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <f t="shared" ref="A7:A48" si="2">A4+7</f>
+        <f t="shared" ref="A7:A48" si="1">A4+7</f>
         <v>44081</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44089</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1">
-        <f t="shared" si="0"/>
-        <v>43857</v>
-      </c>
-      <c r="H7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44083</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44091</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="1">
-        <f t="shared" si="0"/>
-        <v>43496</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44085</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44096</v>
       </c>
       <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" ref="G9:G30" si="3">G7+7</f>
-        <v>43864</v>
-      </c>
-      <c r="H9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44088</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44098</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="1">
-        <f t="shared" si="3"/>
-        <v>43503</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44090</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44103</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" si="3"/>
-        <v>43871</v>
-      </c>
-      <c r="H11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44092</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44105</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" si="3"/>
-        <v>43510</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44095</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44110</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="1">
-        <f t="shared" si="3"/>
-        <v>43878</v>
-      </c>
-      <c r="H13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44097</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44112</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="1">
-        <f t="shared" si="3"/>
-        <v>43517</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44099</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44117</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1">
-        <f t="shared" si="3"/>
-        <v>43885</v>
-      </c>
-      <c r="H15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44102</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44119</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="1">
-        <f t="shared" si="3"/>
-        <v>43524</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44104</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44124</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="1">
-        <f t="shared" si="3"/>
-        <v>43892</v>
-      </c>
-      <c r="H17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44106</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44126</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="1">
-        <f t="shared" si="3"/>
-        <v>43531</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44109</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44131</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="1">
-        <f t="shared" si="3"/>
-        <v>43899</v>
-      </c>
-      <c r="H19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44111</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44133</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="1">
-        <f t="shared" si="3"/>
-        <v>43538</v>
-      </c>
-      <c r="H20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44113</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44138</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="1">
-        <f t="shared" si="3"/>
-        <v>43906</v>
-      </c>
-      <c r="H21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44116</v>
       </c>
       <c r="B22" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44140</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="1">
-        <f t="shared" si="3"/>
-        <v>43545</v>
-      </c>
-      <c r="H22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44118</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44145</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
       </c>
-      <c r="G23" s="1">
-        <f t="shared" si="3"/>
-        <v>43913</v>
-      </c>
-      <c r="H23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44120</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44147</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="1">
-        <f t="shared" si="3"/>
-        <v>43552</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44123</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44152</v>
       </c>
       <c r="E25" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="1">
-        <f t="shared" si="3"/>
-        <v>43920</v>
-      </c>
-      <c r="H25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44125</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44154</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="1">
-        <f t="shared" si="3"/>
-        <v>43559</v>
-      </c>
-      <c r="H26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44127</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44159</v>
       </c>
       <c r="E27" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="1">
-        <f t="shared" si="3"/>
-        <v>43927</v>
-      </c>
-      <c r="H27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44130</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44161</v>
       </c>
       <c r="E28" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="1">
-        <f t="shared" si="3"/>
-        <v>43566</v>
-      </c>
-      <c r="H28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44132</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44166</v>
       </c>
       <c r="E29" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
-        <f t="shared" si="3"/>
-        <v>43934</v>
-      </c>
-      <c r="H29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44134</v>
       </c>
       <c r="B30" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44168</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="1">
-        <f t="shared" si="3"/>
-        <v>43573</v>
-      </c>
-      <c r="H30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44137</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44173</v>
       </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44139</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44175</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
       </c>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44141</v>
       </c>
       <c r="B33" t="s">
@@ -1135,7 +963,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44144</v>
       </c>
       <c r="B34" t="s">
@@ -1146,7 +974,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44146</v>
       </c>
       <c r="B35" t="s">
@@ -1157,7 +985,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44148</v>
       </c>
       <c r="B36" t="s">
@@ -1168,7 +996,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44151</v>
       </c>
       <c r="B37" t="s">
@@ -1179,7 +1007,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44153</v>
       </c>
       <c r="B38" t="s">
@@ -1189,7 +1017,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44155</v>
       </c>
       <c r="B39" t="s">
@@ -1199,7 +1027,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44158</v>
       </c>
       <c r="B40" t="s">
@@ -1209,7 +1037,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44160</v>
       </c>
       <c r="B41" t="s">
@@ -1218,7 +1046,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44162</v>
       </c>
       <c r="B42" t="s">
@@ -1227,7 +1055,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44165</v>
       </c>
       <c r="B43" t="s">
@@ -1236,7 +1064,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44167</v>
       </c>
       <c r="B44" t="s">
@@ -1245,7 +1073,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44169</v>
       </c>
       <c r="B45" t="s">
@@ -1254,7 +1082,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44172</v>
       </c>
       <c r="B46" t="s">
@@ -1263,7 +1091,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44174</v>
       </c>
       <c r="B47" t="s">
@@ -1272,7 +1100,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44176</v>
       </c>
       <c r="B48" t="s">

</xml_diff>